<commit_message>
Last Update 07-02-2019  8:54:02.96
</commit_message>
<xml_diff>
--- a/Acadamic Log Book EVS-18-19.xlsx
+++ b/Acadamic Log Book EVS-18-19.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="116">
   <si>
     <t>S.NO</t>
   </si>
@@ -113,12 +113,6 @@
     <t>Acadamic Year 2018 - 2019</t>
   </si>
   <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
     <t>R.NO</t>
   </si>
   <si>
@@ -375,6 +369,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>AB</t>
   </si>
 </sst>
 </file>
@@ -721,33 +718,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="17" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -757,26 +727,14 @@
     <xf numFmtId="17" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -796,17 +754,44 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -832,19 +817,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="9">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -900,30 +897,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1272,42 +1245,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="54"/>
       <c r="E1" s="18" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="45" t="s">
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="47" t="s">
-        <v>114</v>
-      </c>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="49"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="52"/>
       <c r="Y1" s="22"/>
       <c r="Z1" s="22"/>
       <c r="AA1" s="22"/>
@@ -1320,42 +1293,42 @@
       <c r="AH1" s="22"/>
     </row>
     <row r="2" spans="1:66" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
       <c r="E2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="45" t="s">
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
       <c r="Y2" s="22"/>
       <c r="Z2" s="22"/>
       <c r="AA2" s="22"/>
@@ -1368,42 +1341,42 @@
       <c r="AH2" s="22"/>
     </row>
     <row r="3" spans="1:66" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="35"/>
+      <c r="A3" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="21" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="45" t="s">
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="46" t="s">
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="46"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="46"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
       <c r="Y3" s="23"/>
       <c r="Z3" s="23"/>
       <c r="AA3" s="23"/>
@@ -1416,56 +1389,56 @@
       <c r="AH3" s="23"/>
     </row>
     <row r="4" spans="1:66" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="42">
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="33">
         <v>43070</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="44"/>
-      <c r="Y4" s="42"/>
-      <c r="Z4" s="43"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="43"/>
-      <c r="AC4" s="43"/>
-      <c r="AD4" s="43"/>
-      <c r="AE4" s="43"/>
-      <c r="AF4" s="43"/>
-      <c r="AG4" s="43"/>
-      <c r="AH4" s="43"/>
-      <c r="AI4" s="43"/>
-      <c r="AJ4" s="43"/>
-      <c r="AK4" s="43"/>
-      <c r="AL4" s="43"/>
-      <c r="AM4" s="43"/>
-      <c r="AN4" s="43"/>
-      <c r="AO4" s="43"/>
-      <c r="AP4" s="43"/>
-      <c r="AQ4" s="43"/>
-      <c r="AR4" s="43"/>
-      <c r="AS4" s="43"/>
-      <c r="AT4" s="44"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="35"/>
+      <c r="Y4" s="33"/>
+      <c r="Z4" s="34"/>
+      <c r="AA4" s="34"/>
+      <c r="AB4" s="34"/>
+      <c r="AC4" s="34"/>
+      <c r="AD4" s="34"/>
+      <c r="AE4" s="34"/>
+      <c r="AF4" s="34"/>
+      <c r="AG4" s="34"/>
+      <c r="AH4" s="34"/>
+      <c r="AI4" s="34"/>
+      <c r="AJ4" s="34"/>
+      <c r="AK4" s="34"/>
+      <c r="AL4" s="34"/>
+      <c r="AM4" s="34"/>
+      <c r="AN4" s="34"/>
+      <c r="AO4" s="34"/>
+      <c r="AP4" s="34"/>
+      <c r="AQ4" s="34"/>
+      <c r="AR4" s="34"/>
+      <c r="AS4" s="34"/>
+      <c r="AT4" s="35"/>
       <c r="AU4" s="24"/>
       <c r="AV4" s="24"/>
       <c r="AW4" s="24"/>
@@ -1488,13 +1461,13 @@
       <c r="BN4" s="24"/>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="54" t="s">
+      <c r="B5" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="41" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1574,9 +1547,9 @@
       <c r="BN5" s="31"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="55"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="9" t="s">
         <v>1</v>
       </c>
@@ -1654,11 +1627,11 @@
       <c r="BN6" s="31"/>
     </row>
     <row r="7" spans="1:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" s="56"/>
+        <v>109</v>
+      </c>
+      <c r="C7" s="43"/>
       <c r="D7" s="10" t="s">
         <v>2</v>
       </c>
@@ -1740,10 +1713,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="12" t="s">
@@ -1824,10 +1797,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="27" t="s">
@@ -1908,10 +1881,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="27" t="s">
@@ -1992,10 +1965,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="27" t="s">
@@ -2076,10 +2049,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="27" t="s">
@@ -2160,10 +2133,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="12" t="s">
@@ -2244,10 +2217,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="12" t="s">
@@ -2328,10 +2301,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="12" t="s">
@@ -2412,10 +2385,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="12" t="s">
@@ -2496,10 +2469,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="12" t="s">
@@ -2580,10 +2553,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="12" t="s">
@@ -2664,10 +2637,10 @@
         <v>12</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="12" t="s">
@@ -2748,10 +2721,10 @@
         <v>13</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="12" t="s">
@@ -2832,10 +2805,10 @@
         <v>14</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="27" t="s">
@@ -2916,10 +2889,10 @@
         <v>15</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="27" t="s">
@@ -3000,10 +2973,10 @@
         <v>16</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="12" t="s">
@@ -3084,10 +3057,10 @@
         <v>17</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="27" t="s">
@@ -3168,10 +3141,10 @@
         <v>18</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="12" t="s">
@@ -3252,10 +3225,10 @@
         <v>19</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="12" t="s">
@@ -3336,10 +3309,10 @@
         <v>20</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="12" t="s">
@@ -3420,10 +3393,10 @@
         <v>21</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="12" t="s">
@@ -3504,10 +3477,10 @@
         <v>22</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="12" t="s">
@@ -3588,10 +3561,10 @@
         <v>23</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="12" t="s">
@@ -3672,10 +3645,10 @@
         <v>24</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="12" t="s">
@@ -3756,10 +3729,10 @@
         <v>25</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="27" t="s">
@@ -3840,10 +3813,10 @@
         <v>26</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="12" t="s">
@@ -3924,10 +3897,10 @@
         <v>27</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="12" t="s">
@@ -4008,10 +3981,10 @@
         <v>28</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="27" t="s">
@@ -4092,10 +4065,10 @@
         <v>29</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="12" t="s">
@@ -4176,10 +4149,10 @@
         <v>30</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="12" t="s">
@@ -4260,10 +4233,10 @@
         <v>31</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="12" t="s">
@@ -4344,10 +4317,10 @@
         <v>32</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="12" t="s">
@@ -4428,10 +4401,10 @@
         <v>33</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="27" t="s">
@@ -4512,10 +4485,10 @@
         <v>34</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="27" t="s">
@@ -4596,10 +4569,10 @@
         <v>35</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="12" t="s">
@@ -4680,10 +4653,10 @@
         <v>36</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="27" t="s">
@@ -4764,10 +4737,10 @@
         <v>37</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="27" t="s">
@@ -4848,10 +4821,10 @@
         <v>38</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="12" t="s">
@@ -4932,10 +4905,10 @@
         <v>39</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="12" t="s">
@@ -5012,10 +4985,10 @@
       <c r="BN46" s="32"/>
     </row>
     <row r="47" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="B47" s="52" t="s">
+      <c r="B47" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C47" s="53"/>
+      <c r="C47" s="40"/>
       <c r="D47" s="13"/>
       <c r="E47" s="12">
         <f t="shared" ref="E47:AS47" si="0">COUNTIF(E8:E46,"A")</f>
@@ -5267,10 +5240,10 @@
       </c>
     </row>
     <row r="48" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="B48" s="50" t="s">
+      <c r="B48" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="51"/>
+      <c r="C48" s="37"/>
       <c r="D48" s="13"/>
       <c r="E48" s="12">
         <f>(39-E47)</f>
@@ -5523,12 +5496,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="Y4:AT4"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="E4:X4"/>
@@ -5538,17 +5510,18 @@
     <mergeCell ref="O2:X2"/>
     <mergeCell ref="O3:X3"/>
     <mergeCell ref="O1:X1"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="Y4:AT4"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="E8:BN46">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"OD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5562,7 +5535,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5577,90 +5550,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="64" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65" t="s">
+      <c r="D1" s="60"/>
+      <c r="E1" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+    </row>
+    <row r="2" spans="1:8" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="58"/>
+      <c r="C2" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="60"/>
+      <c r="E2" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-    </row>
-    <row r="2" spans="1:8" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="65" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
     </row>
     <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="64" t="s">
+      <c r="B3" s="59"/>
+      <c r="C3" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="64"/>
-      <c r="E3" s="67" t="s">
+      <c r="D3" s="60"/>
+      <c r="E3" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
-      <c r="B5" s="55"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="19" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="60"/>
-      <c r="B6" s="56"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="19">
         <v>25</v>
       </c>
@@ -5670,254 +5639,282 @@
       <c r="E6" s="19">
         <v>100</v>
       </c>
-      <c r="F6" s="3">
-        <v>50</v>
-      </c>
-      <c r="G6" s="3">
-        <v>50</v>
-      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="28">
         <v>10</v>
       </c>
-      <c r="D7" s="28"/>
+      <c r="D7" s="28">
+        <v>41</v>
+      </c>
       <c r="E7" s="28">
         <f>SUM(C7:D7)</f>
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="28">
         <v>14</v>
       </c>
-      <c r="D8" s="28"/>
+      <c r="D8" s="28">
+        <v>42</v>
+      </c>
       <c r="E8" s="28">
         <f t="shared" ref="E8:E45" si="0">SUM(C8:D8)</f>
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
+        <v>35</v>
+      </c>
+      <c r="C9" s="28">
+        <v>25</v>
+      </c>
+      <c r="D9" s="28">
+        <v>55</v>
+      </c>
       <c r="E9" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C10" s="28">
         <v>24</v>
       </c>
-      <c r="D10" s="28"/>
+      <c r="D10" s="28">
+        <v>58</v>
+      </c>
       <c r="E10" s="28">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="28">
         <v>21</v>
       </c>
-      <c r="D11" s="28"/>
+      <c r="D11" s="28">
+        <v>54</v>
+      </c>
       <c r="E11" s="28">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="28">
         <v>17</v>
       </c>
-      <c r="D12" s="28"/>
+      <c r="D12" s="28">
+        <v>53</v>
+      </c>
       <c r="E12" s="28">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="28">
         <v>15</v>
       </c>
-      <c r="D13" s="28"/>
+      <c r="D13" s="28">
+        <v>37</v>
+      </c>
       <c r="E13" s="28">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="28">
         <v>14</v>
       </c>
-      <c r="D14" s="28"/>
+      <c r="D14" s="28">
+        <v>27</v>
+      </c>
       <c r="E14" s="28">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" s="28">
         <v>24</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="28">
+        <v>64</v>
+      </c>
       <c r="E15" s="28">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" s="28">
         <v>8</v>
       </c>
-      <c r="D16" s="28"/>
+      <c r="D16" s="28">
+        <v>49</v>
+      </c>
       <c r="E16" s="28">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
+        <v>51</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="28">
+        <v>8</v>
+      </c>
       <c r="E17" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="28">
         <v>11</v>
       </c>
-      <c r="D18" s="28"/>
+      <c r="D18" s="28">
+        <v>38</v>
+      </c>
       <c r="E18" s="28">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C19" s="28">
         <v>22</v>
       </c>
-      <c r="D19" s="28"/>
+      <c r="D19" s="28">
+        <v>56</v>
+      </c>
       <c r="E19" s="28">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" s="28">
         <v>3</v>
       </c>
-      <c r="D20" s="28"/>
+      <c r="D20" s="28" t="s">
+        <v>115</v>
+      </c>
       <c r="E20" s="28">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5927,47 +5924,57 @@
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
+        <v>59</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="28">
+        <v>34</v>
+      </c>
       <c r="E21" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="F21" s="28"/>
       <c r="G21" s="28"/>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="28">
         <v>19</v>
       </c>
-      <c r="D22" s="28"/>
+      <c r="D22" s="28">
+        <v>53</v>
+      </c>
       <c r="E22" s="28">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
+        <v>63</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>115</v>
+      </c>
       <c r="E23" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5977,137 +5984,157 @@
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" s="28">
         <v>9</v>
       </c>
-      <c r="D24" s="28"/>
+      <c r="D24" s="28">
+        <v>32</v>
+      </c>
       <c r="E24" s="28">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C25" s="28">
         <v>14</v>
       </c>
-      <c r="D25" s="28"/>
+      <c r="D25" s="28">
+        <v>46</v>
+      </c>
       <c r="E25" s="28">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
+        <v>69</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="28">
+        <v>46</v>
+      </c>
       <c r="E26" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" s="28">
         <v>21</v>
       </c>
-      <c r="D27" s="28"/>
+      <c r="D27" s="28">
+        <v>60</v>
+      </c>
       <c r="E27" s="28">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="F27" s="28"/>
       <c r="G27" s="28"/>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C28" s="28">
         <v>18</v>
       </c>
-      <c r="D28" s="28"/>
+      <c r="D28" s="28">
+        <v>42</v>
+      </c>
       <c r="E28" s="28">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="F28" s="28"/>
       <c r="G28" s="28"/>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C29" s="28">
         <v>19</v>
       </c>
-      <c r="D29" s="28"/>
+      <c r="D29" s="28">
+        <v>51</v>
+      </c>
       <c r="E29" s="28">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
+        <v>77</v>
+      </c>
+      <c r="C30" s="28">
+        <v>15</v>
+      </c>
+      <c r="D30" s="28">
+        <v>58</v>
+      </c>
       <c r="E30" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
     </row>
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C31" s="28">
         <v>17</v>
       </c>
-      <c r="D31" s="28"/>
+      <c r="D31" s="28" t="s">
+        <v>115</v>
+      </c>
       <c r="E31" s="28">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -6117,105 +6144,117 @@
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C32" s="28">
         <v>18</v>
       </c>
-      <c r="D32" s="28"/>
+      <c r="D32" s="28">
+        <v>60</v>
+      </c>
       <c r="E32" s="28">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="F32" s="28"/>
       <c r="G32" s="28"/>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C33" s="28">
         <v>21</v>
       </c>
-      <c r="D33" s="28"/>
+      <c r="D33" s="28">
+        <v>59</v>
+      </c>
       <c r="E33" s="28">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="F33" s="28"/>
       <c r="G33" s="28"/>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C34" s="28">
         <v>12</v>
       </c>
-      <c r="D34" s="28"/>
+      <c r="D34" s="28">
+        <v>38</v>
+      </c>
       <c r="E34" s="28">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="F34" s="28"/>
       <c r="G34" s="28"/>
     </row>
     <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C35" s="28">
         <v>14</v>
       </c>
-      <c r="D35" s="28"/>
+      <c r="D35" s="28">
+        <v>33</v>
+      </c>
       <c r="E35" s="28">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="F35" s="28"/>
       <c r="G35" s="28"/>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C36" s="28">
         <v>19</v>
       </c>
-      <c r="D36" s="28"/>
+      <c r="D36" s="28">
+        <v>65</v>
+      </c>
       <c r="E36" s="28">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="F36" s="28"/>
       <c r="G36" s="28"/>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C37" s="28">
         <v>25</v>
       </c>
-      <c r="D37" s="28"/>
+      <c r="D37" s="28" t="s">
+        <v>115</v>
+      </c>
       <c r="E37" s="28">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -6225,31 +6264,37 @@
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C38" s="28">
         <v>13</v>
       </c>
-      <c r="D38" s="28"/>
+      <c r="D38" s="28">
+        <v>37</v>
+      </c>
       <c r="E38" s="28">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="F38" s="28"/>
       <c r="G38" s="28"/>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
+        <v>95</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>115</v>
+      </c>
       <c r="E39" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6259,113 +6304,129 @@
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
+        <v>97</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="28">
+        <v>35</v>
+      </c>
       <c r="E40" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="F40" s="28"/>
       <c r="G40" s="28"/>
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C41" s="28">
         <v>21</v>
       </c>
-      <c r="D41" s="28"/>
+      <c r="D41" s="28">
+        <v>54</v>
+      </c>
       <c r="E41" s="28">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="F41" s="28"/>
       <c r="G41" s="28"/>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
+        <v>101</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="28">
+        <v>6</v>
+      </c>
       <c r="E42" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F42" s="28"/>
       <c r="G42" s="28"/>
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C43" s="28">
         <v>11</v>
       </c>
-      <c r="D43" s="28"/>
+      <c r="D43" s="28">
+        <v>47</v>
+      </c>
       <c r="E43" s="28">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C44" s="28">
         <v>11</v>
       </c>
-      <c r="D44" s="28"/>
+      <c r="D44" s="28">
+        <v>25</v>
+      </c>
       <c r="E44" s="28">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F44" s="28"/>
       <c r="G44" s="28"/>
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C45" s="28">
         <v>11</v>
       </c>
-      <c r="D45" s="28"/>
+      <c r="D45" s="28">
+        <v>46</v>
+      </c>
       <c r="E45" s="28">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="F45" s="28"/>
       <c r="G45" s="28"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="52" t="s">
+      <c r="A46" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="53"/>
+      <c r="B46" s="40"/>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
       <c r="E46" s="18"/>
@@ -6373,10 +6434,10 @@
       <c r="G46" s="13"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="50" t="s">
+      <c r="A47" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B47" s="51"/>
+      <c r="B47" s="37"/>
       <c r="C47" s="15"/>
       <c r="D47" s="15"/>
       <c r="E47" s="18"/>
@@ -6384,10 +6445,10 @@
       <c r="G47" s="13"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="50" t="s">
+      <c r="A48" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B48" s="51"/>
+      <c r="B48" s="37"/>
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
       <c r="E48" s="18"/>
@@ -6395,10 +6456,10 @@
       <c r="G48" s="13"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="50" t="s">
+      <c r="A49" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="51"/>
+      <c r="B49" s="37"/>
       <c r="C49" s="16"/>
       <c r="D49" s="15"/>
       <c r="E49" s="18"/>
@@ -6407,6 +6468,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -6416,27 +6484,25 @@
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:C45">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="lessThan">
       <formula>12.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D45">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
       <formula>37.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E45">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>50</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:E45">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"AB"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Last Update 07-02-2019 11:43:46.07
</commit_message>
<xml_diff>
--- a/Acadamic Log Book EVS-18-19.xlsx
+++ b/Acadamic Log Book EVS-18-19.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="14535" windowHeight="7695" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="116">
   <si>
     <t>S.NO</t>
   </si>
@@ -834,7 +834,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -842,36 +842,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5518,10 +5488,10 @@
     <mergeCell ref="B5:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="E8:BN46">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"OD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5534,8 +5504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5733,11 +5703,11 @@
         <v>21</v>
       </c>
       <c r="D11" s="28">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E11" s="28">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
@@ -5873,11 +5843,11 @@
         <v>11</v>
       </c>
       <c r="D18" s="28">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E18" s="28">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
@@ -5893,11 +5863,11 @@
         <v>22</v>
       </c>
       <c r="D19" s="28">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E19" s="28">
         <f t="shared" si="0"/>
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
@@ -6029,15 +5999,15 @@
       <c r="B26" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="28" t="s">
-        <v>115</v>
+      <c r="C26" s="28">
+        <v>8</v>
       </c>
       <c r="D26" s="28">
         <v>46</v>
       </c>
       <c r="E26" s="28">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
@@ -6486,17 +6456,17 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:C45">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
       <formula>12.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D45">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>37.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E45">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>